<commit_message>
paso a pc de la pega
sigo mañana
</commit_message>
<xml_diff>
--- a/Resultados/Data_SEN_target.xlsx
+++ b/Resultados/Data_SEN_target.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T327"/>
+  <dimension ref="A1:T332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22328,247 +22328,369 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>STAT_PAZUCAR</t>
-        </is>
-      </c>
-      <c r="B321" t="inlineStr"/>
-      <c r="C321" t="inlineStr"/>
+          <t>CCSS_AMARIA_ALUPAR</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>STATCOM</t>
+          <t>Generador Sincrónico</t>
         </is>
       </c>
       <c r="F321" t="n">
-        <v>1</v>
-      </c>
-      <c r="G321" t="inlineStr"/>
-      <c r="H321" t="inlineStr"/>
-      <c r="I321" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J321" t="n">
-        <v>-0</v>
-      </c>
-      <c r="K321" t="n">
-        <v>36.61</v>
-      </c>
-      <c r="L321" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>LF5</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>00-Norte Grande</t>
+        </is>
+      </c>
+      <c r="I321" t="inlineStr"/>
+      <c r="J321" t="inlineStr"/>
+      <c r="K321" t="inlineStr"/>
+      <c r="L321" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="M321" t="n">
-        <v>100</v>
-      </c>
-      <c r="N321" t="inlineStr"/>
-      <c r="O321" t="inlineStr"/>
-      <c r="P321" t="inlineStr"/>
+        <v>360</v>
+      </c>
+      <c r="N321" t="n">
+        <v>0</v>
+      </c>
+      <c r="O321" t="n">
+        <v>0</v>
+      </c>
+      <c r="P321" t="n">
+        <v>15</v>
+      </c>
       <c r="Q321" t="n">
-        <v>0.575</v>
+        <v>15</v>
       </c>
       <c r="R321" t="n">
-        <v>100</v>
-      </c>
-      <c r="S321" t="n">
-        <v>100</v>
-      </c>
-      <c r="T321" t="n">
-        <v>100</v>
+        <v>360</v>
+      </c>
+      <c r="S321" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T321" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>STAT_POLPAICO</t>
-        </is>
-      </c>
-      <c r="B322" t="inlineStr"/>
-      <c r="C322" t="inlineStr"/>
+          <t>CCSS_AMARIA_TRANSELEC</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>STATCOM</t>
+          <t>Generador Sincrónico</t>
         </is>
       </c>
       <c r="F322" t="n">
-        <v>1</v>
-      </c>
-      <c r="G322" t="inlineStr"/>
-      <c r="H322" t="inlineStr"/>
-      <c r="I322" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J322" t="n">
-        <v>0</v>
-      </c>
-      <c r="K322" t="n">
-        <v>18.45</v>
-      </c>
-      <c r="L322" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>LF7</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>00-Norte Grande</t>
+        </is>
+      </c>
+      <c r="I322" t="inlineStr"/>
+      <c r="J322" t="inlineStr"/>
+      <c r="K322" t="inlineStr"/>
+      <c r="L322" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="M322" t="n">
-        <v>65</v>
-      </c>
-      <c r="N322" t="inlineStr"/>
-      <c r="O322" t="inlineStr"/>
-      <c r="P322" t="inlineStr"/>
+        <v>92</v>
+      </c>
+      <c r="N322" t="n">
+        <v>0</v>
+      </c>
+      <c r="O322" t="n">
+        <v>0</v>
+      </c>
+      <c r="P322" t="n">
+        <v>15</v>
+      </c>
       <c r="Q322" t="n">
-        <v>0.575</v>
+        <v>15</v>
       </c>
       <c r="R322" t="n">
-        <v>65</v>
-      </c>
-      <c r="S322" t="n">
-        <v>65</v>
-      </c>
-      <c r="T322" t="n">
-        <v>65</v>
+        <v>92</v>
+      </c>
+      <c r="S322" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T322" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>ILLAPA_GFM</t>
-        </is>
-      </c>
-      <c r="B323" t="inlineStr"/>
-      <c r="C323" t="inlineStr"/>
+          <t>CCSS_LIKANANTAI_TRANSELEC</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Grid Forming</t>
+          <t>Generador Sincrónico</t>
         </is>
       </c>
       <c r="F323" t="n">
-        <v>1</v>
-      </c>
-      <c r="G323" t="inlineStr"/>
-      <c r="H323" t="inlineStr"/>
-      <c r="I323" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="J323" t="n">
-        <v>100</v>
-      </c>
-      <c r="K323" t="n">
-        <v>9.449999999999999</v>
-      </c>
-      <c r="L323" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>LF6</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>00-Norte Grande</t>
+        </is>
+      </c>
+      <c r="I323" t="inlineStr"/>
+      <c r="J323" t="inlineStr"/>
+      <c r="K323" t="inlineStr"/>
+      <c r="L323" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="M323" t="n">
-        <v>200</v>
-      </c>
-      <c r="N323" t="inlineStr"/>
-      <c r="O323" t="inlineStr"/>
-      <c r="P323" t="inlineStr"/>
+        <v>92</v>
+      </c>
+      <c r="N323" t="n">
+        <v>0</v>
+      </c>
+      <c r="O323" t="n">
+        <v>0</v>
+      </c>
+      <c r="P323" t="n">
+        <v>15</v>
+      </c>
       <c r="Q323" t="n">
-        <v>0.575</v>
+        <v>15</v>
       </c>
       <c r="R323" t="n">
-        <v>200</v>
-      </c>
-      <c r="S323" t="n">
-        <v>200</v>
-      </c>
-      <c r="T323" t="n">
-        <v>200</v>
+        <v>92</v>
+      </c>
+      <c r="S323" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T323" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>LIKANA_GFM</t>
-        </is>
-      </c>
-      <c r="B324" t="inlineStr"/>
-      <c r="C324" t="inlineStr"/>
+          <t>CCSS_ILLAPA_ALUPAR</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Grid Forming</t>
+          <t>Generador Sincrónico</t>
         </is>
       </c>
       <c r="F324" t="n">
-        <v>1</v>
-      </c>
-      <c r="G324" t="inlineStr"/>
-      <c r="H324" t="inlineStr"/>
-      <c r="I324" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J324" t="n">
-        <v>100</v>
-      </c>
-      <c r="K324" t="n">
-        <v>50.06</v>
-      </c>
-      <c r="L324" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>LF4</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>01-Atacama</t>
+        </is>
+      </c>
+      <c r="I324" t="inlineStr"/>
+      <c r="J324" t="inlineStr"/>
+      <c r="K324" t="inlineStr"/>
+      <c r="L324" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="M324" t="n">
-        <v>200</v>
-      </c>
-      <c r="N324" t="inlineStr"/>
-      <c r="O324" t="inlineStr"/>
-      <c r="P324" t="inlineStr"/>
+        <v>270</v>
+      </c>
+      <c r="N324" t="n">
+        <v>0</v>
+      </c>
+      <c r="O324" t="n">
+        <v>0</v>
+      </c>
+      <c r="P324" t="n">
+        <v>15</v>
+      </c>
       <c r="Q324" t="n">
-        <v>0.575</v>
+        <v>15</v>
       </c>
       <c r="R324" t="n">
-        <v>200</v>
-      </c>
-      <c r="S324" t="n">
-        <v>200</v>
-      </c>
-      <c r="T324" t="n">
-        <v>200</v>
+        <v>270</v>
+      </c>
+      <c r="S324" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T324" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>NCHUQUI_GFM</t>
-        </is>
-      </c>
-      <c r="B325" t="inlineStr"/>
-      <c r="C325" t="inlineStr"/>
+          <t>CCSS_TOCOPILLA_ENGIE</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Grid Forming</t>
-        </is>
-      </c>
-      <c r="F325" t="n">
-        <v>1</v>
-      </c>
-      <c r="G325" t="inlineStr"/>
-      <c r="H325" t="inlineStr"/>
-      <c r="I325" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J325" t="n">
-        <v>100</v>
-      </c>
-      <c r="K325" t="n">
-        <v>44.24</v>
-      </c>
-      <c r="L325" t="inlineStr"/>
+          <t>Generador Sincrónico</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>LF4</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>00-Norte Grande</t>
+        </is>
+      </c>
+      <c r="I325" t="inlineStr"/>
+      <c r="J325" t="inlineStr"/>
+      <c r="K325" t="inlineStr"/>
+      <c r="L325" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
       <c r="M325" t="n">
-        <v>200</v>
-      </c>
-      <c r="N325" t="inlineStr"/>
-      <c r="O325" t="inlineStr"/>
-      <c r="P325" t="inlineStr"/>
+        <v>147.1</v>
+      </c>
+      <c r="N325" t="n">
+        <v>0</v>
+      </c>
+      <c r="O325" t="n">
+        <v>0</v>
+      </c>
+      <c r="P325" t="n">
+        <v>15</v>
+      </c>
       <c r="Q325" t="n">
-        <v>0.575</v>
+        <v>13.8</v>
       </c>
       <c r="R325" t="n">
-        <v>200</v>
-      </c>
-      <c r="S325" t="n">
-        <v>200</v>
-      </c>
-      <c r="T325" t="n">
-        <v>200</v>
+        <v>147.1</v>
+      </c>
+      <c r="S325" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T325" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>AMARIA_GFM</t>
+          <t>STAT_PAZUCAR</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -22576,7 +22698,7 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Grid Forming</t>
+          <t>STATCOM</t>
         </is>
       </c>
       <c r="F326" t="n">
@@ -22588,14 +22710,14 @@
         <v>0.6</v>
       </c>
       <c r="J326" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K326" t="n">
-        <v>32.5</v>
+        <v>36.61</v>
       </c>
       <c r="L326" t="inlineStr"/>
       <c r="M326" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N326" t="inlineStr"/>
       <c r="O326" t="inlineStr"/>
@@ -22604,19 +22726,19 @@
         <v>0.575</v>
       </c>
       <c r="R326" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S326" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="T326" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>STAT_CNAVIA</t>
+          <t>STAT_POLPAICO</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -22633,17 +22755,17 @@
       <c r="G327" t="inlineStr"/>
       <c r="H327" t="inlineStr"/>
       <c r="I327" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="J327" t="n">
         <v>0</v>
       </c>
       <c r="K327" t="n">
-        <v>0</v>
+        <v>18.45</v>
       </c>
       <c r="L327" t="inlineStr"/>
       <c r="M327" t="n">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="N327" t="inlineStr"/>
       <c r="O327" t="inlineStr"/>
@@ -22652,12 +22774,252 @@
         <v>0.575</v>
       </c>
       <c r="R327" t="n">
+        <v>65</v>
+      </c>
+      <c r="S327" t="n">
+        <v>65</v>
+      </c>
+      <c r="T327" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>ILLAPA_GFM</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr"/>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="inlineStr"/>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Grid Forming</t>
+        </is>
+      </c>
+      <c r="F328" t="n">
+        <v>0</v>
+      </c>
+      <c r="G328" t="inlineStr"/>
+      <c r="H328" t="inlineStr"/>
+      <c r="I328" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="J328" t="n">
+        <v>0</v>
+      </c>
+      <c r="K328" t="n">
+        <v>0</v>
+      </c>
+      <c r="L328" t="inlineStr"/>
+      <c r="M328" t="n">
+        <v>200</v>
+      </c>
+      <c r="N328" t="inlineStr"/>
+      <c r="O328" t="inlineStr"/>
+      <c r="P328" t="inlineStr"/>
+      <c r="Q328" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="R328" t="n">
+        <v>200</v>
+      </c>
+      <c r="S328" t="n">
+        <v>200</v>
+      </c>
+      <c r="T328" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>LIKANA_GFM</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr"/>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="inlineStr"/>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Grid Forming</t>
+        </is>
+      </c>
+      <c r="F329" t="n">
+        <v>0</v>
+      </c>
+      <c r="G329" t="inlineStr"/>
+      <c r="H329" t="inlineStr"/>
+      <c r="I329" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J329" t="n">
+        <v>0</v>
+      </c>
+      <c r="K329" t="n">
+        <v>0</v>
+      </c>
+      <c r="L329" t="inlineStr"/>
+      <c r="M329" t="n">
+        <v>200</v>
+      </c>
+      <c r="N329" t="inlineStr"/>
+      <c r="O329" t="inlineStr"/>
+      <c r="P329" t="inlineStr"/>
+      <c r="Q329" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="R329" t="n">
+        <v>200</v>
+      </c>
+      <c r="S329" t="n">
+        <v>200</v>
+      </c>
+      <c r="T329" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>NCHUQUI_GFM</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr"/>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr"/>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Grid Forming</t>
+        </is>
+      </c>
+      <c r="F330" t="n">
+        <v>0</v>
+      </c>
+      <c r="G330" t="inlineStr"/>
+      <c r="H330" t="inlineStr"/>
+      <c r="I330" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J330" t="n">
+        <v>0</v>
+      </c>
+      <c r="K330" t="n">
+        <v>0</v>
+      </c>
+      <c r="L330" t="inlineStr"/>
+      <c r="M330" t="n">
+        <v>200</v>
+      </c>
+      <c r="N330" t="inlineStr"/>
+      <c r="O330" t="inlineStr"/>
+      <c r="P330" t="inlineStr"/>
+      <c r="Q330" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="R330" t="n">
+        <v>200</v>
+      </c>
+      <c r="S330" t="n">
+        <v>200</v>
+      </c>
+      <c r="T330" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>AMARIA_GFM</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr"/>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="inlineStr"/>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>Grid Forming</t>
+        </is>
+      </c>
+      <c r="F331" t="n">
+        <v>0</v>
+      </c>
+      <c r="G331" t="inlineStr"/>
+      <c r="H331" t="inlineStr"/>
+      <c r="I331" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J331" t="n">
+        <v>0</v>
+      </c>
+      <c r="K331" t="n">
+        <v>0</v>
+      </c>
+      <c r="L331" t="inlineStr"/>
+      <c r="M331" t="n">
+        <v>200</v>
+      </c>
+      <c r="N331" t="inlineStr"/>
+      <c r="O331" t="inlineStr"/>
+      <c r="P331" t="inlineStr"/>
+      <c r="Q331" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="R331" t="n">
+        <v>200</v>
+      </c>
+      <c r="S331" t="n">
+        <v>200</v>
+      </c>
+      <c r="T331" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>STAT_CNAVIA</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr"/>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="inlineStr"/>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>STATCOM</t>
+        </is>
+      </c>
+      <c r="F332" t="n">
+        <v>1</v>
+      </c>
+      <c r="G332" t="inlineStr"/>
+      <c r="H332" t="inlineStr"/>
+      <c r="I332" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="J332" t="n">
+        <v>0</v>
+      </c>
+      <c r="K332" t="n">
+        <v>0</v>
+      </c>
+      <c r="L332" t="inlineStr"/>
+      <c r="M332" t="n">
         <v>102</v>
       </c>
-      <c r="S327" t="n">
+      <c r="N332" t="inlineStr"/>
+      <c r="O332" t="inlineStr"/>
+      <c r="P332" t="inlineStr"/>
+      <c r="Q332" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="R332" t="n">
         <v>102</v>
       </c>
-      <c r="T327" t="n">
+      <c r="S332" t="n">
+        <v>102</v>
+      </c>
+      <c r="T332" t="n">
         <v>102</v>
       </c>
     </row>

</xml_diff>